<commit_message>
validation is done only for template model
</commit_message>
<xml_diff>
--- a/database/files/prof/business-upload/misc_exception_mapping.xlsx
+++ b/database/files/prof/business-upload/misc_exception_mapping.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="Alternate SL2 Upload" sheetId="1" r:id="rId1"/>
+    <sheet name="Misc Exception" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -422,7 +422,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>